<commit_message>
Travail final et mod exercice 4
</commit_message>
<xml_diff>
--- a/Amine_Fanid_Excel_Exercice04_OperateursFonctionsCond.xlsx
+++ b/Amine_Fanid_Excel_Exercice04_OperateursFonctionsCond.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cvmqc-my.sharepoint.com/personal/e_afanid_etu_cvm_qc_ca/Documents/outils-gestion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cvmqc-my.sharepoint.com/personal/e_afanid_etu_cvm_qc_ca/Documents/outils-gestion/Github/Remises_C13_Amine_Fanid/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="128" documentId="8_{D7874A8A-45C6-4A1E-BFAB-C4B44B4BA468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B77FED16-86FB-451C-A11C-C688C6922069}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-21720" yWindow="7950" windowWidth="21840" windowHeight="13140" xr2:uid="{724B32ED-DB75-4CC6-862E-A7BC0C74707C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{724B32ED-DB75-4CC6-862E-A7BC0C74707C}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultats attendus" sheetId="6" r:id="rId1"/>
@@ -616,7 +615,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00\ &quot;$&quot;"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1671,144 +1670,144 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2157,10 +2156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AK29" sqref="AK29"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="Y5" zoomScale="130" zoomScaleNormal="130" workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="Y5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2186,41 +2182,41 @@
   <sheetData>
     <row r="1" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:34" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="113"/>
-      <c r="AC2" s="113"/>
-      <c r="AD2" s="113"/>
-      <c r="AE2" s="113"/>
-      <c r="AF2" s="113"/>
-      <c r="AG2" s="113"/>
-      <c r="AH2" s="113"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="102"/>
+      <c r="Y2" s="102"/>
+      <c r="Z2" s="102"/>
+      <c r="AA2" s="102"/>
+      <c r="AB2" s="102"/>
+      <c r="AC2" s="102"/>
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="102"/>
+      <c r="AF2" s="102"/>
+      <c r="AG2" s="102"/>
+      <c r="AH2" s="102"/>
     </row>
     <row r="3" spans="2:34" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -2231,122 +2227,122 @@
     </row>
     <row r="4" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:34" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="L5" s="115" t="s">
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="L5" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="R5" s="116" t="s">
+      <c r="M5" s="104"/>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="R5" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="116"/>
-      <c r="Z5" s="116"/>
-      <c r="AA5" s="116"/>
-      <c r="AB5" s="116"/>
-      <c r="AC5" s="116"/>
-      <c r="AD5" s="116"/>
-      <c r="AE5" s="116"/>
-      <c r="AF5" s="116"/>
-      <c r="AG5" s="116"/>
-      <c r="AH5" s="116"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
+      <c r="AC5" s="108"/>
+      <c r="AD5" s="108"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="108"/>
+      <c r="AG5" s="108"/>
+      <c r="AH5" s="108"/>
     </row>
     <row r="6" spans="2:34" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:34" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="123" t="s">
+      <c r="C7" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="119" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="117" t="s">
+      <c r="E7" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="127" t="s">
+      <c r="F7" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="119" t="s">
+      <c r="G7" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="120"/>
-      <c r="I7" s="100" t="s">
+      <c r="H7" s="112"/>
+      <c r="I7" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="101"/>
+      <c r="J7" s="124"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="121" t="s">
+      <c r="L7" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="122"/>
-      <c r="N7" s="121" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="122"/>
-      <c r="P7" s="109" t="s">
+      <c r="M7" s="114"/>
+      <c r="N7" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="114"/>
+      <c r="P7" s="127" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="17"/>
-      <c r="R7" s="102" t="s">
+      <c r="R7" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="103"/>
+      <c r="S7" s="116"/>
       <c r="T7" s="13"/>
-      <c r="U7" s="102" t="s">
+      <c r="U7" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="103"/>
-      <c r="W7" s="102" t="s">
+      <c r="V7" s="116"/>
+      <c r="W7" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="X7" s="103"/>
-      <c r="Y7" s="102" t="s">
+      <c r="X7" s="116"/>
+      <c r="Y7" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="Z7" s="103"/>
-      <c r="AA7" s="102" t="s">
+      <c r="Z7" s="116"/>
+      <c r="AA7" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="AB7" s="103"/>
-      <c r="AC7" s="102" t="s">
+      <c r="AB7" s="116"/>
+      <c r="AC7" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="AD7" s="103"/>
-      <c r="AE7" s="102" t="s">
+      <c r="AD7" s="116"/>
+      <c r="AE7" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="103"/>
+      <c r="AF7" s="116"/>
       <c r="AG7" s="13"/>
-      <c r="AH7" s="111" t="s">
+      <c r="AH7" s="129" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="108"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="128"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="122"/>
       <c r="G8" s="18" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2368,7 @@
       <c r="O8" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="110"/>
+      <c r="P8" s="128"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="25" t="s">
         <v>9</v>
@@ -2418,7 +2414,7 @@
         <v>40</v>
       </c>
       <c r="AG8" s="16"/>
-      <c r="AH8" s="112"/>
+      <c r="AH8" s="130"/>
     </row>
     <row r="9" spans="2:34" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="44" t="s">
@@ -4422,46 +4418,46 @@
       <c r="AH28" s="5"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B29" s="104" t="s">
+      <c r="B29" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="105"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="104" t="s">
+      <c r="C29" s="106"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="106"/>
-      <c r="G29" s="104" t="s">
+      <c r="F29" s="107"/>
+      <c r="G29" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="105"/>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
-      <c r="N29" s="105"/>
-      <c r="O29" s="105"/>
-      <c r="P29" s="106"/>
-      <c r="R29" s="104" t="s">
+      <c r="H29" s="106"/>
+      <c r="I29" s="106"/>
+      <c r="J29" s="106"/>
+      <c r="K29" s="106"/>
+      <c r="L29" s="106"/>
+      <c r="M29" s="106"/>
+      <c r="N29" s="106"/>
+      <c r="O29" s="106"/>
+      <c r="P29" s="107"/>
+      <c r="R29" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="S29" s="105"/>
-      <c r="T29" s="105"/>
-      <c r="U29" s="105"/>
-      <c r="V29" s="105"/>
-      <c r="W29" s="105"/>
-      <c r="X29" s="105"/>
-      <c r="Y29" s="105"/>
-      <c r="Z29" s="105"/>
-      <c r="AA29" s="105"/>
-      <c r="AB29" s="105"/>
-      <c r="AC29" s="105"/>
-      <c r="AD29" s="105"/>
-      <c r="AE29" s="105"/>
-      <c r="AF29" s="105"/>
-      <c r="AG29" s="105"/>
-      <c r="AH29" s="106"/>
+      <c r="S29" s="106"/>
+      <c r="T29" s="106"/>
+      <c r="U29" s="106"/>
+      <c r="V29" s="106"/>
+      <c r="W29" s="106"/>
+      <c r="X29" s="106"/>
+      <c r="Y29" s="106"/>
+      <c r="Z29" s="106"/>
+      <c r="AA29" s="106"/>
+      <c r="AB29" s="106"/>
+      <c r="AC29" s="106"/>
+      <c r="AD29" s="106"/>
+      <c r="AE29" s="106"/>
+      <c r="AF29" s="106"/>
+      <c r="AG29" s="106"/>
+      <c r="AH29" s="107"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="E31" s="10"/>
@@ -4840,6 +4836,16 @@
     <sortCondition ref="AL9"/>
   </sortState>
   <mergeCells count="26">
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="R29:AH29"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AH7:AH8"/>
     <mergeCell ref="B2:AH2"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="L5:P5"/>
@@ -4856,16 +4862,6 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="U7:V7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="R29:AH29"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AH7:AH8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
@@ -4880,10 +4876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AF12" sqref="AF12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5058,7 +5051,7 @@
       </c>
       <c r="E9" s="95">
         <f ca="1">YEARFRAC(D9, TODAY())</f>
-        <v>18.205555555555556</v>
+        <v>18.274999999999999</v>
       </c>
       <c r="F9" s="96">
         <f ca="1">ROUNDDOWN(E9/5,0)+2</f>
@@ -5107,7 +5100,7 @@
         <v>413.00400000000002</v>
       </c>
       <c r="T9" s="92">
-        <f>Q9/$Q$26*100</f>
+        <f t="shared" ref="T9:T26" si="0">Q9/$Q$26*100</f>
         <v>4.917091732151019</v>
       </c>
       <c r="U9" s="92" t="s">
@@ -5145,7 +5138,7 @@
         <f>IF(AND(W9="Oui",Y9="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
-      <c r="AD9" s="133">
+      <c r="AD9" s="100">
         <f>IF(AC9="Oui",((N9-I9)+(O9-J9))*(P9/100),0)</f>
         <v>0</v>
       </c>
@@ -5165,11 +5158,11 @@
         <v>37601</v>
       </c>
       <c r="E10" s="95">
-        <f t="shared" ref="E10:E25" ca="1" si="0">YEARFRAC(D10, TODAY())</f>
-        <v>19.916666666666668</v>
+        <f t="shared" ref="E10:E25" ca="1" si="1">YEARFRAC(D10, TODAY())</f>
+        <v>19.986111111111111</v>
       </c>
       <c r="F10" s="96">
-        <f t="shared" ref="F10:F25" ca="1" si="1">ROUNDDOWN(E10/5,0)+2</f>
+        <f t="shared" ref="F10:F25" ca="1" si="2">ROUNDDOWN(E10/5,0)+2</f>
         <v>5</v>
       </c>
       <c r="G10" s="92">
@@ -5203,26 +5196,26 @@
         <v>2</v>
       </c>
       <c r="Q10" s="92">
-        <f t="shared" ref="Q10:Q26" si="2">SUM(N10:O10)</f>
+        <f t="shared" ref="Q10:Q26" si="3">SUM(N10:O10)</f>
         <v>233697.18</v>
       </c>
       <c r="R10" s="96">
-        <f t="shared" ref="R10:R25" si="3">G10*L10</f>
+        <f t="shared" ref="R10:R25" si="4">G10*L10</f>
         <v>41490</v>
       </c>
       <c r="S10" s="96">
-        <f t="shared" ref="S10:S25" si="4">H10*M10</f>
+        <f t="shared" ref="S10:S25" si="5">H10*M10</f>
         <v>871.41599999999994</v>
       </c>
       <c r="T10" s="92">
-        <f>Q10/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>5.7241742843253718</v>
       </c>
       <c r="U10" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V10" s="97">
-        <f t="shared" ref="V10:V25" si="5">(N10*0.01)+(O10*0.015)</f>
+        <f t="shared" ref="V10:V25" si="6">(N10*0.01)+(O10*0.015)</f>
         <v>3002.9853499999999</v>
       </c>
       <c r="W10" s="96" t="str" cm="1">
@@ -5230,7 +5223,7 @@
         <v>Oui</v>
       </c>
       <c r="X10" s="98">
-        <f t="shared" ref="X10:X25" si="6">IF(W10="oui",(N10-I10)*0.1,0)</f>
+        <f t="shared" ref="X10:X25" si="7">IF(W10="oui",(N10-I10)*0.1,0)</f>
         <v>1438.9979999999996</v>
       </c>
       <c r="Y10" s="96" t="str" cm="1">
@@ -5238,27 +5231,27 @@
         <v>Non</v>
       </c>
       <c r="Z10" s="97">
-        <f t="shared" ref="Z10:Z25" si="7">IF(Y10="Oui",(O10-J10)*0.15,0)</f>
+        <f t="shared" ref="Z10:Z25" si="8">IF(Y10="Oui",(O10-J10)*0.15,0)</f>
         <v>0</v>
       </c>
       <c r="AA10" s="96" t="str">
-        <f t="shared" ref="AA10:AA25" si="8">IF(P10&gt;=6,"Oui","Non")</f>
+        <f t="shared" ref="AA10:AA25" si="9">IF(P10&gt;=6,"Oui","Non")</f>
         <v>Non</v>
       </c>
       <c r="AB10" s="95">
-        <f t="shared" ref="AB10:AB25" si="9">IF(AA10="Oui", (N10+O10)*0.0025, 0)</f>
+        <f t="shared" ref="AB10:AB25" si="10">IF(AA10="Oui", (N10+O10)*0.0025, 0)</f>
         <v>0</v>
       </c>
       <c r="AC10" s="96" t="str">
-        <f t="shared" ref="AC10:AC25" si="10">IF(AND(W10="Oui",Y10="Oui"),"Oui","Non")</f>
-        <v>Non</v>
-      </c>
-      <c r="AD10" s="133">
-        <f t="shared" ref="AD10:AD25" si="11">IF(AC10="Oui",((N10-I10)+(O10-J10))*(P10/100),0)</f>
+        <f t="shared" ref="AC10:AC25" si="11">IF(AND(W10="Oui",Y10="Oui"),"Oui","Non")</f>
+        <v>Non</v>
+      </c>
+      <c r="AD10" s="100">
+        <f t="shared" ref="AD10:AD25" si="12">IF(AC10="Oui",((N10-I10)+(O10-J10))*(P10/100),0)</f>
         <v>0</v>
       </c>
       <c r="AE10" s="96" t="str">
-        <f t="shared" ref="AE10:AE25" si="12">IF(AND(P10&gt;=6)*OR(W10="Oui",Y10="Oui"),"Oui","Non")</f>
+        <f t="shared" ref="AE10:AE25" si="13">IF(AND(P10&gt;=6)*OR(W10="Oui",Y10="Oui"),"Oui","Non")</f>
         <v>Non</v>
       </c>
     </row>
@@ -5273,11 +5266,11 @@
         <v>35826</v>
       </c>
       <c r="E11" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>24.780555555555555</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>24.85</v>
       </c>
       <c r="F11" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="G11" s="92">
@@ -5311,26 +5304,26 @@
         <v>6</v>
       </c>
       <c r="Q11" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>235548.90000000002</v>
       </c>
       <c r="R11" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48492</v>
       </c>
       <c r="S11" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T11" s="92">
-        <f>Q11/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>5.769530278804087</v>
       </c>
       <c r="U11" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V11" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3149.1246500000002</v>
       </c>
       <c r="W11" s="96" t="str" cm="1">
@@ -5338,7 +5331,7 @@
         <v>Non</v>
       </c>
       <c r="X11" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y11" s="96" t="str" cm="1">
@@ -5346,27 +5339,27 @@
         <v>Oui</v>
       </c>
       <c r="Z11" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>365.26349999999945</v>
       </c>
       <c r="AA11" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB11" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>588.87225000000012</v>
       </c>
       <c r="AC11" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD11" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD11" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE11" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Oui</v>
       </c>
     </row>
@@ -5381,11 +5374,11 @@
         <v>35403</v>
       </c>
       <c r="E12" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>25.93611111111111</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>26.005555555555556</v>
       </c>
       <c r="F12" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
       <c r="G12" s="92">
@@ -5419,26 +5412,26 @@
         <v>9</v>
       </c>
       <c r="Q12" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>248390.13</v>
       </c>
       <c r="R12" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>49120.875</v>
       </c>
       <c r="S12" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T12" s="92">
-        <f>Q12/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>6.0840631223116866</v>
       </c>
       <c r="U12" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V12" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3336.7842500000002</v>
       </c>
       <c r="W12" s="96" t="str" cm="1">
@@ -5446,7 +5439,7 @@
         <v>Non</v>
       </c>
       <c r="X12" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y12" s="96" t="str" cm="1">
@@ -5454,27 +5447,27 @@
         <v>Oui</v>
       </c>
       <c r="Z12" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2100.0269999999987</v>
       </c>
       <c r="AA12" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB12" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>620.975325</v>
       </c>
       <c r="AC12" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD12" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD12" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE12" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Oui</v>
       </c>
     </row>
@@ -5489,11 +5482,11 @@
         <v>33093</v>
       </c>
       <c r="E13" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>32.258333333333333</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>32.327777777777776</v>
       </c>
       <c r="F13" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8</v>
       </c>
       <c r="G13" s="92">
@@ -5527,26 +5520,26 @@
         <v>7</v>
       </c>
       <c r="Q13" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>273746</v>
       </c>
       <c r="R13" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56804.25</v>
       </c>
       <c r="S13" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1954.758</v>
       </c>
       <c r="T13" s="92">
-        <f>Q13/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>6.705129320075379</v>
       </c>
       <c r="U13" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V13" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3625.0093999999999</v>
       </c>
       <c r="W13" s="96" t="str" cm="1">
@@ -5554,7 +5547,7 @@
         <v>Oui</v>
       </c>
       <c r="X13" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>519.7349999999991</v>
       </c>
       <c r="Y13" s="96" t="str" cm="1">
@@ -5562,27 +5555,27 @@
         <v>Oui</v>
       </c>
       <c r="Z13" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>801.28049999999928</v>
       </c>
       <c r="AA13" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB13" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>684.36500000000001</v>
       </c>
       <c r="AC13" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Oui</v>
-      </c>
-      <c r="AD13" s="133">
         <f t="shared" si="11"/>
+        <v>Oui</v>
+      </c>
+      <c r="AD13" s="100">
+        <f t="shared" si="12"/>
         <v>737.74539999999911</v>
       </c>
       <c r="AE13" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Oui</v>
       </c>
     </row>
@@ -5597,11 +5590,11 @@
         <v>37900</v>
       </c>
       <c r="E14" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>19.097222222222221</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19.166666666666668</v>
       </c>
       <c r="F14" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
       <c r="G14" s="92">
@@ -5635,26 +5628,26 @@
         <v>6</v>
       </c>
       <c r="Q14" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>206947.46000000002</v>
       </c>
       <c r="R14" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>41160</v>
       </c>
       <c r="S14" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3299.5200000000004</v>
       </c>
       <c r="T14" s="92">
-        <f>Q14/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>5.0689671511588363</v>
       </c>
       <c r="U14" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V14" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2672.39525</v>
       </c>
       <c r="W14" s="96" t="str" cm="1">
@@ -5662,7 +5655,7 @@
         <v>Non</v>
       </c>
       <c r="X14" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y14" s="96" t="str" cm="1">
@@ -5670,27 +5663,27 @@
         <v>Non</v>
       </c>
       <c r="Z14" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA14" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB14" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>517.36865000000012</v>
       </c>
       <c r="AC14" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD14" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD14" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE14" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -5705,11 +5698,11 @@
         <v>35590</v>
       </c>
       <c r="E15" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>25.422222222222221</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>25.491666666666667</v>
       </c>
       <c r="F15" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
       <c r="G15" s="92">
@@ -5743,26 +5736,26 @@
         <v>6</v>
       </c>
       <c r="Q15" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>218334.13</v>
       </c>
       <c r="R15" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48398.25</v>
       </c>
       <c r="S15" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10056.1266</v>
       </c>
       <c r="T15" s="92">
-        <f>Q15/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>5.347872029677692</v>
       </c>
       <c r="U15" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V15" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2780.9497999999999</v>
       </c>
       <c r="W15" s="96" t="str" cm="1">
@@ -5770,7 +5763,7 @@
         <v>Oui</v>
       </c>
       <c r="X15" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1061.7529999999999</v>
       </c>
       <c r="Y15" s="96" t="str" cm="1">
@@ -5778,27 +5771,27 @@
         <v>Non</v>
       </c>
       <c r="Z15" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA15" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB15" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>545.83532500000001</v>
       </c>
       <c r="AC15" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD15" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD15" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE15" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Oui</v>
       </c>
     </row>
@@ -5813,11 +5806,11 @@
         <v>35192</v>
       </c>
       <c r="E16" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>26.511111111111113</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>26.580555555555556</v>
       </c>
       <c r="F16" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
       <c r="G16" s="92">
@@ -5851,26 +5844,26 @@
         <v>4</v>
       </c>
       <c r="Q16" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>254729.35</v>
       </c>
       <c r="R16" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>49931.625</v>
       </c>
       <c r="S16" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4649.0749999999998</v>
       </c>
       <c r="T16" s="92">
-        <f>Q16/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>6.2393358564828096</v>
       </c>
       <c r="U16" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V16" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3371.5443500000001</v>
       </c>
       <c r="W16" s="96" t="str" cm="1">
@@ -5878,7 +5871,7 @@
         <v>Oui</v>
       </c>
       <c r="X16" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>91.553999999999363</v>
       </c>
       <c r="Y16" s="96" t="str" cm="1">
@@ -5886,27 +5879,27 @@
         <v>Oui</v>
       </c>
       <c r="Z16" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>976.15800000000013</v>
       </c>
       <c r="AA16" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Non</v>
       </c>
       <c r="AB16" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AC16" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Oui</v>
-      </c>
-      <c r="AD16" s="133">
         <f t="shared" si="11"/>
+        <v>Oui</v>
+      </c>
+      <c r="AD16" s="100">
+        <f t="shared" si="12"/>
         <v>296.93039999999979</v>
       </c>
       <c r="AE16" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -5921,11 +5914,11 @@
         <v>36628</v>
       </c>
       <c r="E17" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>22.580555555555556</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>22.65</v>
       </c>
       <c r="F17" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="G17" s="92">
@@ -5959,26 +5952,26 @@
         <v>9</v>
       </c>
       <c r="Q17" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>242383.22999999998</v>
       </c>
       <c r="R17" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45342</v>
       </c>
       <c r="S17" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T17" s="92">
-        <f>Q17/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>5.9369302279031437</v>
       </c>
       <c r="U17" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V17" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3172.6669999999999</v>
       </c>
       <c r="W17" s="96" t="str" cm="1">
@@ -5986,7 +5979,7 @@
         <v>Oui</v>
       </c>
       <c r="X17" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>459.24599999999919</v>
       </c>
       <c r="Y17" s="96" t="str" cm="1">
@@ -5994,27 +5987,27 @@
         <v>Oui</v>
       </c>
       <c r="Z17" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>49.552500000000869</v>
       </c>
       <c r="AA17" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB17" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>605.95807500000001</v>
       </c>
       <c r="AC17" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Oui</v>
-      </c>
-      <c r="AD17" s="133">
         <f t="shared" si="11"/>
+        <v>Oui</v>
+      </c>
+      <c r="AD17" s="100">
+        <f t="shared" si="12"/>
         <v>443.05289999999979</v>
       </c>
       <c r="AE17" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Oui</v>
       </c>
     </row>
@@ -6029,11 +6022,11 @@
         <v>30115</v>
       </c>
       <c r="E18" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>40.411111111111111</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>40.480555555555554</v>
       </c>
       <c r="F18" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>10</v>
       </c>
       <c r="G18" s="92">
@@ -6067,26 +6060,26 @@
         <v>5</v>
       </c>
       <c r="Q18" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>255045.78</v>
       </c>
       <c r="R18" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65109</v>
       </c>
       <c r="S18" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8480.1512999999995</v>
       </c>
       <c r="T18" s="92">
-        <f>Q18/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>6.2470864868874596</v>
       </c>
       <c r="U18" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V18" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3392.9933000000001</v>
       </c>
       <c r="W18" s="96" t="str" cm="1">
@@ -6094,7 +6087,7 @@
         <v>Non</v>
       </c>
       <c r="X18" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y18" s="96" t="str" cm="1">
@@ -6102,27 +6095,27 @@
         <v>Non</v>
       </c>
       <c r="Z18" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA18" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Non</v>
       </c>
       <c r="AB18" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AC18" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD18" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD18" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE18" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -6137,12 +6130,12 @@
         <v>41231</v>
       </c>
       <c r="E19" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.9805555555555561</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10.050000000000001</v>
       </c>
       <c r="F19" s="96">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="G19" s="92">
         <v>15.1</v>
@@ -6175,26 +6168,26 @@
         <v>5</v>
       </c>
       <c r="Q19" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>186980.95</v>
       </c>
       <c r="R19" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28312.5</v>
       </c>
       <c r="S19" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T19" s="92">
-        <f>Q19/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>4.5799078347831506</v>
       </c>
       <c r="U19" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V19" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2433.5099499999997</v>
       </c>
       <c r="W19" s="96" t="str" cm="1">
@@ -6202,7 +6195,7 @@
         <v>Non</v>
       </c>
       <c r="X19" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y19" s="96" t="str" cm="1">
@@ -6210,27 +6203,27 @@
         <v>Non</v>
       </c>
       <c r="Z19" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA19" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Non</v>
       </c>
       <c r="AB19" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AC19" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD19" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD19" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE19" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -6245,11 +6238,11 @@
         <v>31824</v>
       </c>
       <c r="E20" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>35.736111111111114</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>35.805555555555557</v>
       </c>
       <c r="F20" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
       <c r="G20" s="92">
@@ -6283,26 +6276,26 @@
         <v>9</v>
       </c>
       <c r="Q20" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>270961.90000000002</v>
       </c>
       <c r="R20" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60260.625</v>
       </c>
       <c r="S20" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7774.6140999999998</v>
       </c>
       <c r="T20" s="92">
-        <f>Q20/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>6.6369356276012539</v>
       </c>
       <c r="U20" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V20" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3610.70795</v>
       </c>
       <c r="W20" s="96" t="str" cm="1">
@@ -6310,7 +6303,7 @@
         <v>Non</v>
       </c>
       <c r="X20" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y20" s="96" t="str" cm="1">
@@ -6318,27 +6311,27 @@
         <v>Oui</v>
       </c>
       <c r="Z20" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>243.4770000000033</v>
       </c>
       <c r="AA20" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB20" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>677.40475000000004</v>
       </c>
       <c r="AC20" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD20" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD20" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE20" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Oui</v>
       </c>
     </row>
@@ -6353,11 +6346,11 @@
         <v>38150</v>
       </c>
       <c r="E21" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>18.413888888888888</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18.483333333333334</v>
       </c>
       <c r="F21" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
       <c r="G21" s="92">
@@ -6391,26 +6384,26 @@
         <v>3</v>
       </c>
       <c r="Q21" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>231401.97999999998</v>
       </c>
       <c r="R21" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40149.375</v>
       </c>
       <c r="S21" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6286.9245000000001</v>
       </c>
       <c r="T21" s="92">
-        <f>Q21/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>5.6679556991572335</v>
       </c>
       <c r="U21" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V21" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3009.6405499999996</v>
       </c>
       <c r="W21" s="96" t="str" cm="1">
@@ -6418,7 +6411,7 @@
         <v>Oui</v>
       </c>
       <c r="X21" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>548.50200000000041</v>
       </c>
       <c r="Y21" s="96" t="str" cm="1">
@@ -6426,27 +6419,27 @@
         <v>Non</v>
       </c>
       <c r="Z21" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA21" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Non</v>
       </c>
       <c r="AB21" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AC21" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD21" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD21" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE21" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -6461,11 +6454,11 @@
         <v>32891</v>
       </c>
       <c r="E22" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>32.81388888888889</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>32.883333333333333</v>
       </c>
       <c r="F22" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>8</v>
       </c>
       <c r="G22" s="92">
@@ -6499,26 +6492,26 @@
         <v>5</v>
       </c>
       <c r="Q22" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>262072.71999999997</v>
       </c>
       <c r="R22" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57580.500000000007</v>
       </c>
       <c r="S22" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7545.0432000000001</v>
       </c>
       <c r="T22" s="92">
-        <f>Q22/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>6.4192042216649909</v>
       </c>
       <c r="U22" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V22" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3528.4550999999997</v>
       </c>
       <c r="W22" s="96" t="str" cm="1">
@@ -6526,7 +6519,7 @@
         <v>Non</v>
       </c>
       <c r="X22" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y22" s="96" t="str" cm="1">
@@ -6534,27 +6527,27 @@
         <v>Oui</v>
       </c>
       <c r="Z22" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1158.424499999998</v>
       </c>
       <c r="AA22" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Non</v>
       </c>
       <c r="AB22" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AC22" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD22" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD22" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE22" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -6569,11 +6562,11 @@
         <v>41102</v>
       </c>
       <c r="E23" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>10.330555555555556</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10.4</v>
       </c>
       <c r="F23" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="G23" s="92">
@@ -6607,26 +6600,26 @@
         <v>9</v>
       </c>
       <c r="Q23" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199348.2</v>
       </c>
       <c r="R23" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28837.5</v>
       </c>
       <c r="S23" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3672.0518999999999</v>
       </c>
       <c r="T23" s="92">
-        <f>Q23/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>4.8828310211811337</v>
       </c>
       <c r="U23" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V23" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2620.8300999999997</v>
       </c>
       <c r="W23" s="96" t="str" cm="1">
@@ -6634,7 +6627,7 @@
         <v>Non</v>
       </c>
       <c r="X23" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y23" s="96" t="str" cm="1">
@@ -6642,27 +6635,27 @@
         <v>Oui</v>
       </c>
       <c r="Z23" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1446.5234999999986</v>
       </c>
       <c r="AA23" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Oui</v>
       </c>
       <c r="AB23" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>498.37050000000005</v>
       </c>
       <c r="AC23" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD23" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD23" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE23" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Oui</v>
       </c>
     </row>
@@ -6677,11 +6670,11 @@
         <v>29465</v>
       </c>
       <c r="E24" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>42.194444444444443</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>42.263888888888886</v>
       </c>
       <c r="F24" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>10</v>
       </c>
       <c r="G24" s="92">
@@ -6715,26 +6708,26 @@
         <v>2</v>
       </c>
       <c r="Q24" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>292684.26</v>
       </c>
       <c r="R24" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67452</v>
       </c>
       <c r="S24" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T24" s="92">
-        <f>Q24/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>7.1690027004981447</v>
       </c>
       <c r="U24" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V24" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3971.6017000000002</v>
       </c>
       <c r="W24" s="96" t="str" cm="1">
@@ -6742,7 +6735,7 @@
         <v>Non</v>
       </c>
       <c r="X24" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y24" s="96" t="str" cm="1">
@@ -6750,27 +6743,27 @@
         <v>Oui</v>
       </c>
       <c r="Z24" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2376.2640000000015</v>
       </c>
       <c r="AA24" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Non</v>
       </c>
       <c r="AB24" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AC24" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD24" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD24" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE24" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -6785,11 +6778,11 @@
         <v>30711</v>
       </c>
       <c r="E25" s="95">
-        <f t="shared" ca="1" si="0"/>
-        <v>38.780555555555559</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>38.85</v>
       </c>
       <c r="F25" s="96">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
       <c r="G25" s="92">
@@ -6823,26 +6816,26 @@
         <v>5</v>
       </c>
       <c r="Q25" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>269616.54000000004</v>
       </c>
       <c r="R25" s="96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64378.125</v>
       </c>
       <c r="S25" s="96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12957.444299999999</v>
       </c>
       <c r="T25" s="92">
-        <f>Q25/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>6.6039824053366125</v>
       </c>
       <c r="U25" s="92" t="s">
         <v>72</v>
       </c>
       <c r="V25" s="97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3552.8549500000004</v>
       </c>
       <c r="W25" s="96" t="str" cm="1">
@@ -6850,7 +6843,7 @@
         <v>Oui</v>
       </c>
       <c r="X25" s="98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>481.38899999999995</v>
       </c>
       <c r="Y25" s="96" t="str" cm="1">
@@ -6858,27 +6851,27 @@
         <v>Non</v>
       </c>
       <c r="Z25" s="97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA25" s="96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Non</v>
       </c>
       <c r="AB25" s="95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AC25" s="96" t="str">
-        <f t="shared" si="10"/>
-        <v>Non</v>
-      </c>
-      <c r="AD25" s="133">
         <f t="shared" si="11"/>
+        <v>Non</v>
+      </c>
+      <c r="AD25" s="100">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE25" s="96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Non</v>
       </c>
     </row>
@@ -6900,7 +6893,7 @@
         <v>2596154.92</v>
       </c>
       <c r="Q26" s="92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4082635.65</v>
       </c>
       <c r="R26" s="92">
@@ -6912,27 +6905,27 @@
         <v>67960.128899999996</v>
       </c>
       <c r="T26" s="92">
-        <f>Q26/$Q$26*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="V26" s="134">
+      <c r="V26" s="101">
         <f>SUM(V9:V25)</f>
         <v>53807.131099999991</v>
       </c>
-      <c r="X26" s="134">
-        <f t="shared" ref="X26" si="13">SUM(X9:X25)</f>
+      <c r="X26" s="101">
+        <f t="shared" ref="X26" si="14">SUM(X9:X25)</f>
         <v>4659.7329999999974</v>
       </c>
-      <c r="Z26" s="134">
-        <f t="shared" ref="Z26" si="14">SUM(Z9:Z25)</f>
+      <c r="Z26" s="101">
+        <f t="shared" ref="Z26" si="15">SUM(Z9:Z25)</f>
         <v>9516.9704999999994</v>
       </c>
-      <c r="AB26" s="134">
-        <f t="shared" ref="AB26" si="15">SUM(AB9:AB25)</f>
+      <c r="AB26" s="101">
+        <f t="shared" ref="AB26" si="16">SUM(AB9:AB25)</f>
         <v>5241.0172250000005</v>
       </c>
-      <c r="AD26" s="134">
-        <f t="shared" ref="AD26" si="16">SUM(AD9:AD25)</f>
+      <c r="AD26" s="101">
+        <f t="shared" ref="AD26" si="17">SUM(AD9:AD25)</f>
         <v>1477.7286999999988</v>
       </c>
     </row>
@@ -6985,10 +6978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7002,15 +6992,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="131" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="130" t="s">
+      <c r="C4" s="132" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="88" t="s">
@@ -7018,25 +7008,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="131"/>
+      <c r="C5" s="133"/>
       <c r="D5" s="70" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="131"/>
+      <c r="C6" s="133"/>
       <c r="D6" s="71" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="131"/>
+      <c r="C7" s="133"/>
       <c r="D7" s="70" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="132"/>
+      <c r="C8" s="134"/>
       <c r="D8" s="89" t="s">
         <v>56</v>
       </c>
@@ -7056,7 +7046,7 @@
       <c r="C11" s="72"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="132" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="88" t="s">
@@ -7064,43 +7054,43 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="131"/>
+      <c r="C13" s="133"/>
       <c r="D13" s="70" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="131"/>
+      <c r="C14" s="133"/>
       <c r="D14" s="68" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="131"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="87" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="131"/>
+      <c r="C16" s="133"/>
       <c r="D16" s="68" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="131"/>
+      <c r="C17" s="133"/>
       <c r="D17" s="87" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="131"/>
+      <c r="C18" s="133"/>
       <c r="D18" s="68" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="132"/>
+      <c r="C19" s="134"/>
       <c r="D19" s="89" t="s">
         <v>61</v>
       </c>

</xml_diff>